<commit_message>
Updates to R and stan code for symbol consistency
</commit_message>
<xml_diff>
--- a/output/processed/sofa/SOFA_posterior_sums.xlsx
+++ b/output/processed/sofa/SOFA_posterior_sums.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/26362cec7e0913ab/Documents/Papers/Monterey_mussel_urchin_otter/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nhydra-my.sharepoint.com/personal/ttinker_nhydra-eco_com/Documents/Nhydra/Projects/Aquarium/Ecosystem/ecosystem_coupling/output/processed/sofa/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="51" documentId="8_{111E843A-5537-4657-A4BF-263839D9392E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B4D83BF2-1AA8-476F-A4E9-B6B40C43B125}"/>
+  <xr:revisionPtr revIDLastSave="59" documentId="8_{111E843A-5537-4657-A4BF-263839D9392E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{412E5E20-98BB-4855-B888-7602F7E15441}"/>
   <bookViews>
     <workbookView xWindow="5610" yWindow="2790" windowWidth="38700" windowHeight="15345" xr2:uid="{6A775A36-9EC4-4E96-B058-46638B27D0E2}"/>
   </bookViews>
@@ -86,13 +86,13 @@
     <t>tau</t>
   </si>
   <si>
-    <t>pi</t>
+    <t>mu_est</t>
   </si>
   <si>
-    <t>V_mu</t>
+    <t>eta</t>
   </si>
   <si>
-    <t>mu_est</t>
+    <t>sig_mu</t>
   </si>
 </sst>
 </file>
@@ -470,8 +470,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BCFC25A-3074-4E72-9557-C6179F155635}">
   <dimension ref="A1:D449"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="A193" workbookViewId="0">
+      <selection activeCell="A211" sqref="A211:A221"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -495,7 +495,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B2">
         <v>2006</v>
@@ -509,7 +509,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B3">
         <v>2007</v>
@@ -523,7 +523,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B4">
         <v>2008</v>
@@ -537,7 +537,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B5">
         <v>2009</v>
@@ -551,7 +551,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B6">
         <v>2010</v>
@@ -565,7 +565,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B7">
         <v>2011</v>
@@ -579,7 +579,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B8">
         <v>2012</v>
@@ -593,7 +593,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B9">
         <v>2013</v>
@@ -607,7 +607,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B10">
         <v>2014</v>
@@ -621,7 +621,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B11">
         <v>2015</v>
@@ -635,7 +635,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B12">
         <v>2016</v>
@@ -649,7 +649,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B13">
         <v>2017</v>
@@ -663,7 +663,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B14">
         <v>2018</v>
@@ -677,7 +677,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B15">
         <v>2019</v>
@@ -691,7 +691,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B16">
         <v>2020</v>
@@ -705,7 +705,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B17">
         <v>2021</v>
@@ -719,7 +719,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B18">
         <v>2022</v>
@@ -733,7 +733,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B19">
         <v>2023</v>
@@ -747,7 +747,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B20">
         <v>2024</v>
@@ -761,7 +761,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B21">
         <v>2006</v>
@@ -775,7 +775,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B22">
         <v>2007</v>
@@ -789,7 +789,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B23">
         <v>2008</v>
@@ -803,7 +803,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B24">
         <v>2009</v>
@@ -817,7 +817,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B25">
         <v>2010</v>
@@ -831,7 +831,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B26">
         <v>2011</v>
@@ -845,7 +845,7 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B27">
         <v>2012</v>
@@ -859,7 +859,7 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B28">
         <v>2013</v>
@@ -873,7 +873,7 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B29">
         <v>2014</v>
@@ -887,7 +887,7 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B30">
         <v>2015</v>
@@ -901,7 +901,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B31">
         <v>2016</v>
@@ -915,7 +915,7 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B32">
         <v>2017</v>
@@ -929,7 +929,7 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B33">
         <v>2018</v>
@@ -943,7 +943,7 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B34">
         <v>2019</v>
@@ -957,7 +957,7 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B35">
         <v>2020</v>
@@ -971,7 +971,7 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B36">
         <v>2021</v>
@@ -985,7 +985,7 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B37">
         <v>2022</v>
@@ -999,7 +999,7 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B38">
         <v>2023</v>
@@ -1013,7 +1013,7 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B39">
         <v>2024</v>
@@ -1027,7 +1027,7 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B40">
         <v>2006</v>
@@ -1041,7 +1041,7 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B41">
         <v>2007</v>
@@ -1055,7 +1055,7 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B42">
         <v>2008</v>
@@ -1069,7 +1069,7 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B43">
         <v>2009</v>
@@ -1083,7 +1083,7 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B44">
         <v>2010</v>
@@ -1097,7 +1097,7 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B45">
         <v>2011</v>
@@ -1111,7 +1111,7 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B46">
         <v>2012</v>
@@ -1125,7 +1125,7 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B47">
         <v>2013</v>
@@ -1139,7 +1139,7 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B48">
         <v>2014</v>
@@ -1153,7 +1153,7 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B49">
         <v>2015</v>
@@ -1167,7 +1167,7 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B50">
         <v>2016</v>
@@ -1181,7 +1181,7 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B51">
         <v>2017</v>
@@ -1195,7 +1195,7 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B52">
         <v>2018</v>
@@ -1209,7 +1209,7 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B53">
         <v>2019</v>
@@ -1223,7 +1223,7 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B54">
         <v>2020</v>
@@ -1237,7 +1237,7 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B55">
         <v>2021</v>
@@ -1251,7 +1251,7 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B56">
         <v>2022</v>
@@ -1265,7 +1265,7 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B57">
         <v>2023</v>
@@ -1279,7 +1279,7 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B58">
         <v>2024</v>
@@ -1293,7 +1293,7 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B59">
         <v>2006</v>
@@ -1307,7 +1307,7 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B60">
         <v>2007</v>
@@ -1321,7 +1321,7 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B61">
         <v>2008</v>
@@ -1335,7 +1335,7 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B62">
         <v>2009</v>
@@ -1349,7 +1349,7 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B63">
         <v>2010</v>
@@ -1363,7 +1363,7 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B64">
         <v>2011</v>
@@ -1377,7 +1377,7 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B65">
         <v>2012</v>
@@ -1391,7 +1391,7 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B66">
         <v>2013</v>
@@ -1405,7 +1405,7 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B67">
         <v>2014</v>
@@ -1419,7 +1419,7 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B68">
         <v>2015</v>
@@ -1433,7 +1433,7 @@
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B69">
         <v>2016</v>
@@ -1447,7 +1447,7 @@
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B70">
         <v>2017</v>
@@ -1461,7 +1461,7 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B71">
         <v>2018</v>
@@ -1475,7 +1475,7 @@
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B72">
         <v>2019</v>
@@ -1489,7 +1489,7 @@
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B73">
         <v>2020</v>
@@ -1503,7 +1503,7 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B74">
         <v>2021</v>
@@ -1517,7 +1517,7 @@
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B75">
         <v>2022</v>
@@ -1531,7 +1531,7 @@
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B76">
         <v>2023</v>
@@ -1545,7 +1545,7 @@
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B77">
         <v>2024</v>
@@ -1559,7 +1559,7 @@
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B78">
         <v>2006</v>
@@ -1573,7 +1573,7 @@
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B79">
         <v>2007</v>
@@ -1587,7 +1587,7 @@
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B80">
         <v>2008</v>
@@ -1601,7 +1601,7 @@
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B81">
         <v>2009</v>
@@ -1615,7 +1615,7 @@
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B82">
         <v>2010</v>
@@ -1629,7 +1629,7 @@
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B83">
         <v>2011</v>
@@ -1643,7 +1643,7 @@
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B84">
         <v>2012</v>
@@ -1657,7 +1657,7 @@
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B85">
         <v>2013</v>
@@ -1671,7 +1671,7 @@
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B86">
         <v>2014</v>
@@ -1685,7 +1685,7 @@
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B87">
         <v>2015</v>
@@ -1699,7 +1699,7 @@
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B88">
         <v>2016</v>
@@ -1713,7 +1713,7 @@
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B89">
         <v>2017</v>
@@ -1727,7 +1727,7 @@
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B90">
         <v>2018</v>
@@ -1741,7 +1741,7 @@
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B91">
         <v>2019</v>
@@ -1755,7 +1755,7 @@
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B92">
         <v>2020</v>
@@ -1769,7 +1769,7 @@
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B93">
         <v>2021</v>
@@ -1783,7 +1783,7 @@
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B94">
         <v>2022</v>
@@ -1797,7 +1797,7 @@
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B95">
         <v>2023</v>
@@ -1811,7 +1811,7 @@
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B96">
         <v>2024</v>
@@ -1825,7 +1825,7 @@
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B97">
         <v>2006</v>
@@ -1839,7 +1839,7 @@
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B98">
         <v>2007</v>
@@ -1853,7 +1853,7 @@
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B99">
         <v>2008</v>
@@ -1867,7 +1867,7 @@
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B100">
         <v>2009</v>
@@ -1881,7 +1881,7 @@
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B101">
         <v>2010</v>
@@ -1895,7 +1895,7 @@
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B102">
         <v>2011</v>
@@ -1909,7 +1909,7 @@
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B103">
         <v>2012</v>
@@ -1923,7 +1923,7 @@
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B104">
         <v>2013</v>
@@ -1937,7 +1937,7 @@
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B105">
         <v>2014</v>
@@ -1951,7 +1951,7 @@
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B106">
         <v>2015</v>
@@ -1965,7 +1965,7 @@
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B107">
         <v>2016</v>
@@ -1979,7 +1979,7 @@
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B108">
         <v>2017</v>
@@ -1993,7 +1993,7 @@
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B109">
         <v>2018</v>
@@ -2007,7 +2007,7 @@
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B110">
         <v>2019</v>
@@ -2021,7 +2021,7 @@
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B111">
         <v>2020</v>
@@ -2035,7 +2035,7 @@
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B112">
         <v>2021</v>
@@ -2049,7 +2049,7 @@
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B113">
         <v>2022</v>
@@ -2063,7 +2063,7 @@
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B114">
         <v>2023</v>
@@ -2077,7 +2077,7 @@
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B115">
         <v>2024</v>
@@ -2091,7 +2091,7 @@
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B116">
         <v>2006</v>
@@ -2105,7 +2105,7 @@
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B117">
         <v>2007</v>
@@ -2119,7 +2119,7 @@
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B118">
         <v>2008</v>
@@ -2133,7 +2133,7 @@
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B119">
         <v>2009</v>
@@ -2147,7 +2147,7 @@
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B120">
         <v>2010</v>
@@ -2161,7 +2161,7 @@
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B121">
         <v>2011</v>
@@ -2175,7 +2175,7 @@
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B122">
         <v>2012</v>
@@ -2189,7 +2189,7 @@
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B123">
         <v>2013</v>
@@ -2203,7 +2203,7 @@
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B124">
         <v>2014</v>
@@ -2217,7 +2217,7 @@
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B125">
         <v>2015</v>
@@ -2231,7 +2231,7 @@
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B126">
         <v>2016</v>
@@ -2245,7 +2245,7 @@
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B127">
         <v>2017</v>
@@ -2259,7 +2259,7 @@
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B128">
         <v>2018</v>
@@ -2273,7 +2273,7 @@
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B129">
         <v>2019</v>
@@ -2287,7 +2287,7 @@
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B130">
         <v>2020</v>
@@ -2301,7 +2301,7 @@
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B131">
         <v>2021</v>
@@ -2315,7 +2315,7 @@
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B132">
         <v>2022</v>
@@ -2329,7 +2329,7 @@
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B133">
         <v>2023</v>
@@ -2343,7 +2343,7 @@
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B134">
         <v>2024</v>
@@ -2357,7 +2357,7 @@
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B135">
         <v>2006</v>
@@ -2371,7 +2371,7 @@
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B136">
         <v>2007</v>
@@ -2385,7 +2385,7 @@
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B137">
         <v>2008</v>
@@ -2399,7 +2399,7 @@
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B138">
         <v>2009</v>
@@ -2413,7 +2413,7 @@
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B139">
         <v>2010</v>
@@ -2427,7 +2427,7 @@
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B140">
         <v>2011</v>
@@ -2441,7 +2441,7 @@
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B141">
         <v>2012</v>
@@ -2455,7 +2455,7 @@
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B142">
         <v>2013</v>
@@ -2469,7 +2469,7 @@
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B143">
         <v>2014</v>
@@ -2483,7 +2483,7 @@
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B144">
         <v>2015</v>
@@ -2497,7 +2497,7 @@
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B145">
         <v>2016</v>
@@ -2511,7 +2511,7 @@
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B146">
         <v>2017</v>
@@ -2525,7 +2525,7 @@
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B147">
         <v>2018</v>
@@ -2539,7 +2539,7 @@
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B148">
         <v>2019</v>
@@ -2553,7 +2553,7 @@
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B149">
         <v>2020</v>
@@ -2567,7 +2567,7 @@
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B150">
         <v>2021</v>
@@ -2581,7 +2581,7 @@
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B151">
         <v>2022</v>
@@ -2595,7 +2595,7 @@
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B152">
         <v>2023</v>
@@ -2609,7 +2609,7 @@
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B153">
         <v>2024</v>
@@ -2623,7 +2623,7 @@
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B154">
         <v>2006</v>
@@ -2637,7 +2637,7 @@
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B155">
         <v>2007</v>
@@ -2651,7 +2651,7 @@
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B156">
         <v>2008</v>
@@ -2665,7 +2665,7 @@
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B157">
         <v>2009</v>
@@ -2679,7 +2679,7 @@
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B158">
         <v>2010</v>
@@ -2693,7 +2693,7 @@
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B159">
         <v>2011</v>
@@ -2707,7 +2707,7 @@
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B160">
         <v>2012</v>
@@ -2721,7 +2721,7 @@
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B161">
         <v>2013</v>
@@ -2735,7 +2735,7 @@
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B162">
         <v>2014</v>
@@ -2749,7 +2749,7 @@
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B163">
         <v>2015</v>
@@ -2763,7 +2763,7 @@
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B164">
         <v>2016</v>
@@ -2777,7 +2777,7 @@
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B165">
         <v>2017</v>
@@ -2791,7 +2791,7 @@
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B166">
         <v>2018</v>
@@ -2805,7 +2805,7 @@
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B167">
         <v>2019</v>
@@ -2819,7 +2819,7 @@
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B168">
         <v>2020</v>
@@ -2833,7 +2833,7 @@
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B169">
         <v>2021</v>
@@ -2847,7 +2847,7 @@
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B170">
         <v>2022</v>
@@ -2861,7 +2861,7 @@
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B171">
         <v>2023</v>
@@ -2875,7 +2875,7 @@
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B172">
         <v>2024</v>
@@ -2889,7 +2889,7 @@
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B173">
         <v>2006</v>
@@ -2903,7 +2903,7 @@
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B174">
         <v>2007</v>
@@ -2917,7 +2917,7 @@
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B175">
         <v>2008</v>
@@ -2931,7 +2931,7 @@
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B176">
         <v>2009</v>
@@ -2945,7 +2945,7 @@
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B177">
         <v>2010</v>
@@ -2959,7 +2959,7 @@
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B178">
         <v>2011</v>
@@ -2973,7 +2973,7 @@
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B179">
         <v>2012</v>
@@ -2987,7 +2987,7 @@
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B180">
         <v>2013</v>
@@ -3001,7 +3001,7 @@
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B181">
         <v>2014</v>
@@ -3015,7 +3015,7 @@
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B182">
         <v>2015</v>
@@ -3029,7 +3029,7 @@
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B183">
         <v>2016</v>
@@ -3043,7 +3043,7 @@
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B184">
         <v>2017</v>
@@ -3057,7 +3057,7 @@
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B185">
         <v>2018</v>
@@ -3071,7 +3071,7 @@
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B186">
         <v>2019</v>
@@ -3085,7 +3085,7 @@
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B187">
         <v>2020</v>
@@ -3099,7 +3099,7 @@
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B188">
         <v>2021</v>
@@ -3113,7 +3113,7 @@
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B189">
         <v>2022</v>
@@ -3127,7 +3127,7 @@
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B190">
         <v>2023</v>
@@ -3141,7 +3141,7 @@
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B191">
         <v>2024</v>
@@ -3155,7 +3155,7 @@
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B192">
         <v>2006</v>
@@ -3169,7 +3169,7 @@
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B193">
         <v>2007</v>
@@ -3183,7 +3183,7 @@
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B194">
         <v>2008</v>
@@ -3197,7 +3197,7 @@
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B195">
         <v>2009</v>
@@ -3211,7 +3211,7 @@
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B196">
         <v>2010</v>
@@ -3225,7 +3225,7 @@
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B197">
         <v>2011</v>
@@ -3239,7 +3239,7 @@
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B198">
         <v>2012</v>
@@ -3253,7 +3253,7 @@
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B199">
         <v>2013</v>
@@ -3267,7 +3267,7 @@
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B200">
         <v>2014</v>
@@ -3281,7 +3281,7 @@
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B201">
         <v>2015</v>
@@ -3295,7 +3295,7 @@
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B202">
         <v>2016</v>
@@ -3309,7 +3309,7 @@
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B203">
         <v>2017</v>
@@ -3323,7 +3323,7 @@
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B204">
         <v>2018</v>
@@ -3337,7 +3337,7 @@
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B205">
         <v>2019</v>
@@ -3351,7 +3351,7 @@
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B206">
         <v>2020</v>
@@ -3365,7 +3365,7 @@
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B207">
         <v>2021</v>
@@ -3379,7 +3379,7 @@
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B208">
         <v>2022</v>
@@ -3393,7 +3393,7 @@
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B209">
         <v>2023</v>
@@ -3407,7 +3407,7 @@
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B210">
         <v>2024</v>
@@ -3421,128 +3421,128 @@
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C211" t="s">
         <v>3</v>
       </c>
       <c r="D211">
-        <v>1.4908862589086001E-2</v>
+        <v>0.12210185334009473</v>
       </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C212" t="s">
         <v>4</v>
       </c>
       <c r="D212">
-        <v>1.3663268949481701E-2</v>
+        <v>0.11688998652357567</v>
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C213" t="s">
         <v>5</v>
       </c>
       <c r="D213">
-        <v>1.7428562363429399E-2</v>
+        <v>0.13201728054853046</v>
       </c>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C214" t="s">
         <v>6</v>
       </c>
       <c r="D214">
-        <v>1.4306904219304299E-2</v>
+        <v>0.11961147193854066</v>
       </c>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C215" t="s">
         <v>7</v>
       </c>
       <c r="D215">
-        <v>1.5920757289145999E-2</v>
+        <v>0.1261774832890005</v>
       </c>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C216" t="s">
         <v>8</v>
       </c>
       <c r="D216">
-        <v>1.9905040860066201E-2</v>
+        <v>0.14108522552013092</v>
       </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C217" t="s">
         <v>9</v>
       </c>
       <c r="D217">
-        <v>2.2208744189938501E-2</v>
+        <v>0.14902598494872799</v>
       </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C218" t="s">
         <v>10</v>
       </c>
       <c r="D218">
-        <v>1.6724522235118802E-2</v>
+        <v>0.12932332440483735</v>
       </c>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C219" t="s">
         <v>11</v>
       </c>
       <c r="D219">
-        <v>2.4278947927376199E-2</v>
+        <v>0.15581703349562331</v>
       </c>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C220" t="s">
         <v>12</v>
       </c>
       <c r="D220">
-        <v>9.9429368259218096E-3</v>
+        <v>9.97142759384122E-2</v>
       </c>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C221" t="s">
         <v>13</v>
       </c>
       <c r="D221">
-        <v>1.31863409798241E-2</v>
+        <v>0.11483179428983986</v>
       </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B222">
         <v>2006</v>
@@ -3556,7 +3556,7 @@
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B223">
         <v>2007</v>
@@ -3570,7 +3570,7 @@
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B224">
         <v>2008</v>
@@ -3584,7 +3584,7 @@
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B225">
         <v>2009</v>
@@ -3598,7 +3598,7 @@
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B226">
         <v>2010</v>
@@ -3612,7 +3612,7 @@
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B227">
         <v>2011</v>
@@ -3626,7 +3626,7 @@
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B228">
         <v>2012</v>
@@ -3640,7 +3640,7 @@
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B229">
         <v>2013</v>
@@ -3654,7 +3654,7 @@
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B230">
         <v>2014</v>
@@ -3668,7 +3668,7 @@
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B231">
         <v>2015</v>
@@ -3682,7 +3682,7 @@
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B232">
         <v>2016</v>
@@ -3696,7 +3696,7 @@
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B233">
         <v>2017</v>
@@ -3710,7 +3710,7 @@
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B234">
         <v>2018</v>
@@ -3724,7 +3724,7 @@
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B235">
         <v>2019</v>
@@ -3738,7 +3738,7 @@
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B236">
         <v>2020</v>
@@ -3752,7 +3752,7 @@
     </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B237">
         <v>2021</v>
@@ -3766,7 +3766,7 @@
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B238">
         <v>2022</v>
@@ -3780,7 +3780,7 @@
     </row>
     <row r="239" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B239">
         <v>2023</v>
@@ -3794,7 +3794,7 @@
     </row>
     <row r="240" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B240">
         <v>2024</v>
@@ -3808,7 +3808,7 @@
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B241">
         <v>2006</v>
@@ -3822,7 +3822,7 @@
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B242">
         <v>2007</v>
@@ -3836,7 +3836,7 @@
     </row>
     <row r="243" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B243">
         <v>2008</v>
@@ -3850,7 +3850,7 @@
     </row>
     <row r="244" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B244">
         <v>2009</v>
@@ -3864,7 +3864,7 @@
     </row>
     <row r="245" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B245">
         <v>2010</v>
@@ -3878,7 +3878,7 @@
     </row>
     <row r="246" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B246">
         <v>2011</v>
@@ -3892,7 +3892,7 @@
     </row>
     <row r="247" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B247">
         <v>2012</v>
@@ -3906,7 +3906,7 @@
     </row>
     <row r="248" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B248">
         <v>2013</v>
@@ -3920,7 +3920,7 @@
     </row>
     <row r="249" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B249">
         <v>2014</v>
@@ -3934,7 +3934,7 @@
     </row>
     <row r="250" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B250">
         <v>2015</v>
@@ -3948,7 +3948,7 @@
     </row>
     <row r="251" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B251">
         <v>2016</v>
@@ -3962,7 +3962,7 @@
     </row>
     <row r="252" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B252">
         <v>2017</v>
@@ -3976,7 +3976,7 @@
     </row>
     <row r="253" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B253">
         <v>2018</v>
@@ -3990,7 +3990,7 @@
     </row>
     <row r="254" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B254">
         <v>2019</v>
@@ -4004,7 +4004,7 @@
     </row>
     <row r="255" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B255">
         <v>2020</v>
@@ -4018,7 +4018,7 @@
     </row>
     <row r="256" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B256">
         <v>2021</v>
@@ -4032,7 +4032,7 @@
     </row>
     <row r="257" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B257">
         <v>2022</v>
@@ -4046,7 +4046,7 @@
     </row>
     <row r="258" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B258">
         <v>2023</v>
@@ -4060,7 +4060,7 @@
     </row>
     <row r="259" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B259">
         <v>2024</v>
@@ -4074,7 +4074,7 @@
     </row>
     <row r="260" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B260">
         <v>2006</v>
@@ -4088,7 +4088,7 @@
     </row>
     <row r="261" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B261">
         <v>2007</v>
@@ -4102,7 +4102,7 @@
     </row>
     <row r="262" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B262">
         <v>2008</v>
@@ -4116,7 +4116,7 @@
     </row>
     <row r="263" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B263">
         <v>2009</v>
@@ -4130,7 +4130,7 @@
     </row>
     <row r="264" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B264">
         <v>2010</v>
@@ -4144,7 +4144,7 @@
     </row>
     <row r="265" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B265">
         <v>2011</v>
@@ -4158,7 +4158,7 @@
     </row>
     <row r="266" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B266">
         <v>2012</v>
@@ -4172,7 +4172,7 @@
     </row>
     <row r="267" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B267">
         <v>2013</v>
@@ -4186,7 +4186,7 @@
     </row>
     <row r="268" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B268">
         <v>2014</v>
@@ -4200,7 +4200,7 @@
     </row>
     <row r="269" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B269">
         <v>2015</v>
@@ -4214,7 +4214,7 @@
     </row>
     <row r="270" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B270">
         <v>2016</v>
@@ -4228,7 +4228,7 @@
     </row>
     <row r="271" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B271">
         <v>2017</v>
@@ -4242,7 +4242,7 @@
     </row>
     <row r="272" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B272">
         <v>2018</v>
@@ -4256,7 +4256,7 @@
     </row>
     <row r="273" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B273">
         <v>2019</v>
@@ -4270,7 +4270,7 @@
     </row>
     <row r="274" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B274">
         <v>2020</v>
@@ -4284,7 +4284,7 @@
     </row>
     <row r="275" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B275">
         <v>2021</v>
@@ -4298,7 +4298,7 @@
     </row>
     <row r="276" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B276">
         <v>2022</v>
@@ -4312,7 +4312,7 @@
     </row>
     <row r="277" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B277">
         <v>2023</v>
@@ -4326,7 +4326,7 @@
     </row>
     <row r="278" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B278">
         <v>2024</v>
@@ -4340,7 +4340,7 @@
     </row>
     <row r="279" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B279">
         <v>2006</v>
@@ -4354,7 +4354,7 @@
     </row>
     <row r="280" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B280">
         <v>2007</v>
@@ -4368,7 +4368,7 @@
     </row>
     <row r="281" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B281">
         <v>2008</v>
@@ -4382,7 +4382,7 @@
     </row>
     <row r="282" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B282">
         <v>2009</v>
@@ -4396,7 +4396,7 @@
     </row>
     <row r="283" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B283">
         <v>2010</v>
@@ -4410,7 +4410,7 @@
     </row>
     <row r="284" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B284">
         <v>2011</v>
@@ -4424,7 +4424,7 @@
     </row>
     <row r="285" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B285">
         <v>2012</v>
@@ -4438,7 +4438,7 @@
     </row>
     <row r="286" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B286">
         <v>2013</v>
@@ -4452,7 +4452,7 @@
     </row>
     <row r="287" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B287">
         <v>2014</v>
@@ -4466,7 +4466,7 @@
     </row>
     <row r="288" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B288">
         <v>2015</v>
@@ -4480,7 +4480,7 @@
     </row>
     <row r="289" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B289">
         <v>2016</v>
@@ -4494,7 +4494,7 @@
     </row>
     <row r="290" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B290">
         <v>2017</v>
@@ -4508,7 +4508,7 @@
     </row>
     <row r="291" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B291">
         <v>2018</v>
@@ -4522,7 +4522,7 @@
     </row>
     <row r="292" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A292" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B292">
         <v>2019</v>
@@ -4536,7 +4536,7 @@
     </row>
     <row r="293" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A293" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B293">
         <v>2020</v>
@@ -4550,7 +4550,7 @@
     </row>
     <row r="294" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A294" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B294">
         <v>2021</v>
@@ -4564,7 +4564,7 @@
     </row>
     <row r="295" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A295" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B295">
         <v>2022</v>
@@ -4578,7 +4578,7 @@
     </row>
     <row r="296" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A296" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B296">
         <v>2023</v>
@@ -4592,7 +4592,7 @@
     </row>
     <row r="297" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A297" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B297">
         <v>2024</v>
@@ -4606,7 +4606,7 @@
     </row>
     <row r="298" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A298" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B298">
         <v>2006</v>
@@ -4620,7 +4620,7 @@
     </row>
     <row r="299" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A299" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B299">
         <v>2007</v>
@@ -4634,7 +4634,7 @@
     </row>
     <row r="300" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A300" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B300">
         <v>2008</v>
@@ -4648,7 +4648,7 @@
     </row>
     <row r="301" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A301" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B301">
         <v>2009</v>
@@ -4662,7 +4662,7 @@
     </row>
     <row r="302" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A302" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B302">
         <v>2010</v>
@@ -4676,7 +4676,7 @@
     </row>
     <row r="303" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A303" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B303">
         <v>2011</v>
@@ -4690,7 +4690,7 @@
     </row>
     <row r="304" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A304" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B304">
         <v>2012</v>
@@ -4704,7 +4704,7 @@
     </row>
     <row r="305" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A305" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B305">
         <v>2013</v>
@@ -4718,7 +4718,7 @@
     </row>
     <row r="306" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A306" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B306">
         <v>2014</v>
@@ -4732,7 +4732,7 @@
     </row>
     <row r="307" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A307" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B307">
         <v>2015</v>
@@ -4746,7 +4746,7 @@
     </row>
     <row r="308" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A308" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B308">
         <v>2016</v>
@@ -4760,7 +4760,7 @@
     </row>
     <row r="309" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A309" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B309">
         <v>2017</v>
@@ -4774,7 +4774,7 @@
     </row>
     <row r="310" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A310" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B310">
         <v>2018</v>
@@ -4788,7 +4788,7 @@
     </row>
     <row r="311" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A311" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B311">
         <v>2019</v>
@@ -4802,7 +4802,7 @@
     </row>
     <row r="312" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A312" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B312">
         <v>2020</v>
@@ -4816,7 +4816,7 @@
     </row>
     <row r="313" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A313" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B313">
         <v>2021</v>
@@ -4830,7 +4830,7 @@
     </row>
     <row r="314" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A314" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B314">
         <v>2022</v>
@@ -4844,7 +4844,7 @@
     </row>
     <row r="315" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A315" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B315">
         <v>2023</v>
@@ -4858,7 +4858,7 @@
     </row>
     <row r="316" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A316" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B316">
         <v>2024</v>
@@ -4872,7 +4872,7 @@
     </row>
     <row r="317" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A317" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B317">
         <v>2006</v>
@@ -4886,7 +4886,7 @@
     </row>
     <row r="318" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A318" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B318">
         <v>2007</v>
@@ -4900,7 +4900,7 @@
     </row>
     <row r="319" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A319" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B319">
         <v>2008</v>
@@ -4914,7 +4914,7 @@
     </row>
     <row r="320" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A320" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B320">
         <v>2009</v>
@@ -4928,7 +4928,7 @@
     </row>
     <row r="321" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A321" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B321">
         <v>2010</v>
@@ -4942,7 +4942,7 @@
     </row>
     <row r="322" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A322" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B322">
         <v>2011</v>
@@ -4956,7 +4956,7 @@
     </row>
     <row r="323" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A323" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B323">
         <v>2012</v>
@@ -4970,7 +4970,7 @@
     </row>
     <row r="324" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A324" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B324">
         <v>2013</v>
@@ -4984,7 +4984,7 @@
     </row>
     <row r="325" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A325" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B325">
         <v>2014</v>
@@ -4998,7 +4998,7 @@
     </row>
     <row r="326" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A326" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B326">
         <v>2015</v>
@@ -5012,7 +5012,7 @@
     </row>
     <row r="327" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A327" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B327">
         <v>2016</v>
@@ -5026,7 +5026,7 @@
     </row>
     <row r="328" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A328" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B328">
         <v>2017</v>
@@ -5040,7 +5040,7 @@
     </row>
     <row r="329" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A329" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B329">
         <v>2018</v>
@@ -5054,7 +5054,7 @@
     </row>
     <row r="330" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A330" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B330">
         <v>2019</v>
@@ -5068,7 +5068,7 @@
     </row>
     <row r="331" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A331" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B331">
         <v>2020</v>
@@ -5082,7 +5082,7 @@
     </row>
     <row r="332" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A332" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B332">
         <v>2021</v>
@@ -5096,7 +5096,7 @@
     </row>
     <row r="333" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A333" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B333">
         <v>2022</v>
@@ -5110,7 +5110,7 @@
     </row>
     <row r="334" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A334" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B334">
         <v>2023</v>
@@ -5124,7 +5124,7 @@
     </row>
     <row r="335" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A335" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B335">
         <v>2024</v>
@@ -5138,7 +5138,7 @@
     </row>
     <row r="336" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A336" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B336">
         <v>2006</v>
@@ -5152,7 +5152,7 @@
     </row>
     <row r="337" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A337" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B337">
         <v>2007</v>
@@ -5166,7 +5166,7 @@
     </row>
     <row r="338" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A338" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B338">
         <v>2008</v>
@@ -5180,7 +5180,7 @@
     </row>
     <row r="339" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A339" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B339">
         <v>2009</v>
@@ -5194,7 +5194,7 @@
     </row>
     <row r="340" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A340" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B340">
         <v>2010</v>
@@ -5208,7 +5208,7 @@
     </row>
     <row r="341" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A341" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B341">
         <v>2011</v>
@@ -5222,7 +5222,7 @@
     </row>
     <row r="342" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A342" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B342">
         <v>2012</v>
@@ -5236,7 +5236,7 @@
     </row>
     <row r="343" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A343" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B343">
         <v>2013</v>
@@ -5250,7 +5250,7 @@
     </row>
     <row r="344" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A344" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B344">
         <v>2014</v>
@@ -5264,7 +5264,7 @@
     </row>
     <row r="345" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A345" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B345">
         <v>2015</v>
@@ -5278,7 +5278,7 @@
     </row>
     <row r="346" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A346" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B346">
         <v>2016</v>
@@ -5292,7 +5292,7 @@
     </row>
     <row r="347" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A347" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B347">
         <v>2017</v>
@@ -5306,7 +5306,7 @@
     </row>
     <row r="348" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A348" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B348">
         <v>2018</v>
@@ -5320,7 +5320,7 @@
     </row>
     <row r="349" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A349" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B349">
         <v>2019</v>
@@ -5334,7 +5334,7 @@
     </row>
     <row r="350" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A350" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B350">
         <v>2020</v>
@@ -5348,7 +5348,7 @@
     </row>
     <row r="351" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A351" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B351">
         <v>2021</v>
@@ -5362,7 +5362,7 @@
     </row>
     <row r="352" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A352" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B352">
         <v>2022</v>
@@ -5376,7 +5376,7 @@
     </row>
     <row r="353" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A353" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B353">
         <v>2023</v>
@@ -5390,7 +5390,7 @@
     </row>
     <row r="354" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A354" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B354">
         <v>2024</v>
@@ -5404,7 +5404,7 @@
     </row>
     <row r="355" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A355" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B355">
         <v>2006</v>
@@ -5418,7 +5418,7 @@
     </row>
     <row r="356" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A356" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B356">
         <v>2007</v>
@@ -5432,7 +5432,7 @@
     </row>
     <row r="357" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A357" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B357">
         <v>2008</v>
@@ -5446,7 +5446,7 @@
     </row>
     <row r="358" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A358" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B358">
         <v>2009</v>
@@ -5460,7 +5460,7 @@
     </row>
     <row r="359" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A359" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B359">
         <v>2010</v>
@@ -5474,7 +5474,7 @@
     </row>
     <row r="360" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A360" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B360">
         <v>2011</v>
@@ -5488,7 +5488,7 @@
     </row>
     <row r="361" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A361" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B361">
         <v>2012</v>
@@ -5502,7 +5502,7 @@
     </row>
     <row r="362" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A362" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B362">
         <v>2013</v>
@@ -5516,7 +5516,7 @@
     </row>
     <row r="363" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A363" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B363">
         <v>2014</v>
@@ -5530,7 +5530,7 @@
     </row>
     <row r="364" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A364" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B364">
         <v>2015</v>
@@ -5544,7 +5544,7 @@
     </row>
     <row r="365" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A365" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B365">
         <v>2016</v>
@@ -5558,7 +5558,7 @@
     </row>
     <row r="366" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A366" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B366">
         <v>2017</v>
@@ -5572,7 +5572,7 @@
     </row>
     <row r="367" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A367" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B367">
         <v>2018</v>
@@ -5586,7 +5586,7 @@
     </row>
     <row r="368" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A368" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B368">
         <v>2019</v>
@@ -5600,7 +5600,7 @@
     </row>
     <row r="369" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A369" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B369">
         <v>2020</v>
@@ -5614,7 +5614,7 @@
     </row>
     <row r="370" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A370" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B370">
         <v>2021</v>
@@ -5628,7 +5628,7 @@
     </row>
     <row r="371" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A371" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B371">
         <v>2022</v>
@@ -5642,7 +5642,7 @@
     </row>
     <row r="372" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A372" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B372">
         <v>2023</v>
@@ -5656,7 +5656,7 @@
     </row>
     <row r="373" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A373" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B373">
         <v>2024</v>
@@ -5670,7 +5670,7 @@
     </row>
     <row r="374" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A374" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B374">
         <v>2006</v>
@@ -5684,7 +5684,7 @@
     </row>
     <row r="375" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A375" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B375">
         <v>2007</v>
@@ -5698,7 +5698,7 @@
     </row>
     <row r="376" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A376" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B376">
         <v>2008</v>
@@ -5712,7 +5712,7 @@
     </row>
     <row r="377" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A377" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B377">
         <v>2009</v>
@@ -5726,7 +5726,7 @@
     </row>
     <row r="378" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A378" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B378">
         <v>2010</v>
@@ -5740,7 +5740,7 @@
     </row>
     <row r="379" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A379" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B379">
         <v>2011</v>
@@ -5754,7 +5754,7 @@
     </row>
     <row r="380" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A380" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B380">
         <v>2012</v>
@@ -5768,7 +5768,7 @@
     </row>
     <row r="381" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A381" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B381">
         <v>2013</v>
@@ -5782,7 +5782,7 @@
     </row>
     <row r="382" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A382" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B382">
         <v>2014</v>
@@ -5796,7 +5796,7 @@
     </row>
     <row r="383" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A383" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B383">
         <v>2015</v>
@@ -5810,7 +5810,7 @@
     </row>
     <row r="384" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A384" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B384">
         <v>2016</v>
@@ -5824,7 +5824,7 @@
     </row>
     <row r="385" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A385" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B385">
         <v>2017</v>
@@ -5838,7 +5838,7 @@
     </row>
     <row r="386" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A386" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B386">
         <v>2018</v>
@@ -5852,7 +5852,7 @@
     </row>
     <row r="387" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A387" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B387">
         <v>2019</v>
@@ -5866,7 +5866,7 @@
     </row>
     <row r="388" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A388" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B388">
         <v>2020</v>
@@ -5880,7 +5880,7 @@
     </row>
     <row r="389" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A389" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B389">
         <v>2021</v>
@@ -5894,7 +5894,7 @@
     </row>
     <row r="390" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A390" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B390">
         <v>2022</v>
@@ -5908,7 +5908,7 @@
     </row>
     <row r="391" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A391" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B391">
         <v>2023</v>
@@ -5922,7 +5922,7 @@
     </row>
     <row r="392" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A392" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B392">
         <v>2024</v>
@@ -5936,7 +5936,7 @@
     </row>
     <row r="393" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A393" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B393">
         <v>2006</v>
@@ -5950,7 +5950,7 @@
     </row>
     <row r="394" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A394" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B394">
         <v>2007</v>
@@ -5964,7 +5964,7 @@
     </row>
     <row r="395" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A395" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B395">
         <v>2008</v>
@@ -5978,7 +5978,7 @@
     </row>
     <row r="396" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A396" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B396">
         <v>2009</v>
@@ -5992,7 +5992,7 @@
     </row>
     <row r="397" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A397" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B397">
         <v>2010</v>
@@ -6006,7 +6006,7 @@
     </row>
     <row r="398" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A398" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B398">
         <v>2011</v>
@@ -6020,7 +6020,7 @@
     </row>
     <row r="399" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A399" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B399">
         <v>2012</v>
@@ -6034,7 +6034,7 @@
     </row>
     <row r="400" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A400" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B400">
         <v>2013</v>
@@ -6048,7 +6048,7 @@
     </row>
     <row r="401" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A401" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B401">
         <v>2014</v>
@@ -6062,7 +6062,7 @@
     </row>
     <row r="402" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A402" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B402">
         <v>2015</v>
@@ -6076,7 +6076,7 @@
     </row>
     <row r="403" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A403" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B403">
         <v>2016</v>
@@ -6090,7 +6090,7 @@
     </row>
     <row r="404" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A404" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B404">
         <v>2017</v>
@@ -6104,7 +6104,7 @@
     </row>
     <row r="405" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A405" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B405">
         <v>2018</v>
@@ -6118,7 +6118,7 @@
     </row>
     <row r="406" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A406" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B406">
         <v>2019</v>
@@ -6132,7 +6132,7 @@
     </row>
     <row r="407" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A407" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B407">
         <v>2020</v>
@@ -6146,7 +6146,7 @@
     </row>
     <row r="408" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A408" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B408">
         <v>2021</v>
@@ -6160,7 +6160,7 @@
     </row>
     <row r="409" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A409" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B409">
         <v>2022</v>
@@ -6174,7 +6174,7 @@
     </row>
     <row r="410" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A410" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B410">
         <v>2023</v>
@@ -6188,7 +6188,7 @@
     </row>
     <row r="411" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A411" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B411">
         <v>2024</v>
@@ -6202,7 +6202,7 @@
     </row>
     <row r="412" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A412" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B412">
         <v>2006</v>
@@ -6216,7 +6216,7 @@
     </row>
     <row r="413" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A413" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B413">
         <v>2007</v>
@@ -6230,7 +6230,7 @@
     </row>
     <row r="414" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A414" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B414">
         <v>2008</v>
@@ -6244,7 +6244,7 @@
     </row>
     <row r="415" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A415" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B415">
         <v>2009</v>
@@ -6258,7 +6258,7 @@
     </row>
     <row r="416" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A416" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B416">
         <v>2010</v>
@@ -6272,7 +6272,7 @@
     </row>
     <row r="417" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A417" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B417">
         <v>2011</v>
@@ -6286,7 +6286,7 @@
     </row>
     <row r="418" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A418" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B418">
         <v>2012</v>
@@ -6300,7 +6300,7 @@
     </row>
     <row r="419" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A419" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B419">
         <v>2013</v>
@@ -6314,7 +6314,7 @@
     </row>
     <row r="420" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A420" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B420">
         <v>2014</v>
@@ -6328,7 +6328,7 @@
     </row>
     <row r="421" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A421" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B421">
         <v>2015</v>
@@ -6342,7 +6342,7 @@
     </row>
     <row r="422" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A422" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B422">
         <v>2016</v>
@@ -6356,7 +6356,7 @@
     </row>
     <row r="423" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A423" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B423">
         <v>2017</v>
@@ -6370,7 +6370,7 @@
     </row>
     <row r="424" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A424" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B424">
         <v>2018</v>
@@ -6384,7 +6384,7 @@
     </row>
     <row r="425" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A425" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B425">
         <v>2019</v>
@@ -6398,7 +6398,7 @@
     </row>
     <row r="426" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A426" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B426">
         <v>2020</v>
@@ -6412,7 +6412,7 @@
     </row>
     <row r="427" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A427" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B427">
         <v>2021</v>
@@ -6426,7 +6426,7 @@
     </row>
     <row r="428" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A428" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B428">
         <v>2022</v>
@@ -6440,7 +6440,7 @@
     </row>
     <row r="429" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A429" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B429">
         <v>2023</v>
@@ -6454,7 +6454,7 @@
     </row>
     <row r="430" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A430" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B430">
         <v>2024</v>

</xml_diff>

<commit_message>
Final tweaks to code
</commit_message>
<xml_diff>
--- a/output/processed/sofa/SOFA_posterior_sums.xlsx
+++ b/output/processed/sofa/SOFA_posterior_sums.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nhydra-my.sharepoint.com/personal/ttinker_nhydra-eco_com/Documents/Nhydra/Projects/Aquarium/Ecosystem/ecosystem_coupling/output/processed/sofa/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="59" documentId="8_{111E843A-5537-4657-A4BF-263839D9392E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{412E5E20-98BB-4855-B888-7602F7E15441}"/>
+  <xr:revisionPtr revIDLastSave="60" documentId="8_{111E843A-5537-4657-A4BF-263839D9392E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DF45975E-27DC-44F1-9C62-5A9B932D8EBD}"/>
   <bookViews>
-    <workbookView xWindow="5610" yWindow="2790" windowWidth="38700" windowHeight="15345" xr2:uid="{6A775A36-9EC4-4E96-B058-46638B27D0E2}"/>
+    <workbookView xWindow="5100" yWindow="960" windowWidth="43995" windowHeight="17250" xr2:uid="{6A775A36-9EC4-4E96-B058-46638B27D0E2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -470,8 +470,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BCFC25A-3074-4E72-9557-C6179F155635}">
   <dimension ref="A1:D449"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A193" workbookViewId="0">
-      <selection activeCell="A211" sqref="A211:A221"/>
+    <sheetView tabSelected="1" topLeftCell="A121" workbookViewId="0">
+      <selection activeCell="D146" sqref="D146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2506,7 +2506,7 @@
         <v>10</v>
       </c>
       <c r="D145">
-        <v>1.80102132189472</v>
+        <v>1.5010213218947199</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>